<commit_message>
Fixed issue with retry analyser not update returned tests in qTest; CSA Workflow Alerts scenario updated; If I Logout of the Hub I Expect to be Logged out of Moodle Totara scenario added; HUB - My Learning scenario updated (simplified way to fill field with JS); data-provider-thread-count in productFactory.xml updated to 4; data-provider-thread-count in smoke.xml updated to 3; i_set_text_with_js step definition created;
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13035"/>
+    <workbookView windowWidth="24345" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Tag</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>BPPAUATUSER</t>
+    <t>BPPADMINUSER</t>
   </si>
   <si>
     <t>automation@bpp.com.noahuat</t>
@@ -37,82 +37,22 @@
     <t>descr.</t>
   </si>
   <si>
-    <t>BPPUATPASSWORD</t>
+    <t>BPPADMINPASSWORD</t>
   </si>
   <si>
     <t>Welcome1@</t>
   </si>
   <si>
-    <t>YAHOOEMAILCASEUSER</t>
-  </si>
-  <si>
-    <t>casemail777</t>
-  </si>
-  <si>
-    <t>YAHOOEMAILCASEPASSWORD</t>
-  </si>
-  <si>
-    <t>Casemail123</t>
-  </si>
-  <si>
-    <t>VLENOAHSTUDENTONE</t>
-  </si>
-  <si>
-    <t>student081601</t>
-  </si>
-  <si>
-    <t>VLENOAHTEACHERONE</t>
-  </si>
-  <si>
-    <t>teacher081602</t>
-  </si>
-  <si>
-    <t>VLENOAHPASS</t>
-  </si>
-  <si>
-    <t>Welcome1!</t>
-  </si>
-  <si>
-    <t>VLENOAHSTUDENTTWO</t>
-  </si>
-  <si>
-    <t>student081603</t>
-  </si>
-  <si>
-    <t>VLEPQSTUDENTONE</t>
-  </si>
-  <si>
-    <t>n.fusionk</t>
-  </si>
-  <si>
-    <t>VLEPQSTUDENTTWO</t>
-  </si>
-  <si>
-    <t>h.fivo</t>
-  </si>
-  <si>
-    <t>VLEPQPASS</t>
-  </si>
-  <si>
-    <t>BPPuat01!</t>
-  </si>
-  <si>
-    <t>VLENOAHSTUDENTTHREE</t>
-  </si>
-  <si>
-    <t>student081602</t>
-  </si>
-  <si>
-    <t>YAHOOEMAILUSER</t>
-  </si>
-  <si>
-    <t>ayaks.spam</t>
-  </si>
-  <si>
-    <t>YAHOOEMAILPASSWORD</t>
-  </si>
-  <si>
-    <t>Qwerty2@</t>
+    <t>YAHOOEMAILCSAUSER</t>
+  </si>
+  <si>
+    <t>nadineanja@yahoo.com</t>
+  </si>
+  <si>
+    <t>YAHOOEMAILCSAPASSWORD</t>
+  </si>
+  <si>
+    <t>Wake Up 19!</t>
   </si>
   <si>
     <t>BPPBANNERUSER</t>
@@ -189,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -226,6 +166,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -233,14 +188,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,9 +202,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,44 +211,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,8 +262,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,38 +272,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,187 +310,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,6 +517,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -586,17 +541,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,26 +567,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,168 +606,161 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -843,12 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1170,13 +1104,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71428571428571" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.71428571428571" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="33.8571428571429" style="5" customWidth="1"/>
     <col min="2" max="2" width="45.4285714285714" style="5" customWidth="1"/>
@@ -1239,135 +1173,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
+    <row r="6" s="7" customFormat="1" spans="1:3">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" s="7" customFormat="1" spans="1:3">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" s="7" customFormat="1" spans="1:3">
-      <c r="A14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" s="7" customFormat="1" spans="1:3">
-      <c r="A15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" s="7" customFormat="1" spans="1:3">
-      <c r="A16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" s="7" customFormat="1" spans="1:3">
-      <c r="A17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1410,10 +1234,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1421,10 +1245,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1432,10 +1256,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1477,10 +1301,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1488,10 +1312,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1499,10 +1323,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1510,10 +1334,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -1521,10 +1345,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
@@ -1572,10 +1396,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1583,10 +1407,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
added test for Scorm completion assignment
</commit_message>
<xml_diff>
--- a/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
+++ b/src/main/resources/data/bpp/keywords.metadata/metadata/UAT/Common_MetaData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28200" windowHeight="13035"/>
+    <workbookView windowWidth="24345" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>Tag</t>
   </si>
@@ -28,7 +28,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>BPPAUATUSER</t>
+    <t>BPPADMINUSER</t>
   </si>
   <si>
     <t>automation@bpp.com.noahuat</t>
@@ -37,82 +37,22 @@
     <t>descr.</t>
   </si>
   <si>
-    <t>BPPUATPASSWORD</t>
+    <t>BPPADMINPASSWORD</t>
   </si>
   <si>
     <t>Welcome1@</t>
   </si>
   <si>
-    <t>YAHOOEMAILCASEUSER</t>
-  </si>
-  <si>
-    <t>casemail777</t>
-  </si>
-  <si>
-    <t>YAHOOEMAILCASEPASSWORD</t>
-  </si>
-  <si>
-    <t>Casemail123</t>
-  </si>
-  <si>
-    <t>VLENOAHSTUDENTONE</t>
-  </si>
-  <si>
-    <t>student081601</t>
-  </si>
-  <si>
-    <t>VLENOAHTEACHERONE</t>
-  </si>
-  <si>
-    <t>teacher081602</t>
-  </si>
-  <si>
-    <t>VLENOAHPASS</t>
-  </si>
-  <si>
-    <t>Welcome1!</t>
-  </si>
-  <si>
-    <t>VLENOAHSTUDENTTWO</t>
-  </si>
-  <si>
-    <t>student081603</t>
-  </si>
-  <si>
-    <t>VLEPQSTUDENTONE</t>
-  </si>
-  <si>
-    <t>n.fusionk</t>
-  </si>
-  <si>
-    <t>VLEPQSTUDENTTWO</t>
-  </si>
-  <si>
-    <t>h.fivo</t>
-  </si>
-  <si>
-    <t>VLEPQPASS</t>
-  </si>
-  <si>
-    <t>BPPuat01!</t>
-  </si>
-  <si>
-    <t>VLENOAHSTUDENTTHREE</t>
-  </si>
-  <si>
-    <t>student081602</t>
-  </si>
-  <si>
-    <t>YAHOOEMAILUSER</t>
-  </si>
-  <si>
-    <t>ayaks.spam</t>
-  </si>
-  <si>
-    <t>YAHOOEMAILPASSWORD</t>
-  </si>
-  <si>
-    <t>Qwerty2@</t>
+    <t>YAHOOEMAILCSAUSER</t>
+  </si>
+  <si>
+    <t>nadineanja@yahoo.com</t>
+  </si>
+  <si>
+    <t>YAHOOEMAILCSAPASSWORD</t>
+  </si>
+  <si>
+    <t>Wake Up 19!</t>
   </si>
   <si>
     <t>BPPBANNERUSER</t>
@@ -189,10 +129,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -226,6 +166,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -233,14 +188,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -254,9 +202,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,44 +211,44 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,8 +262,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,38 +272,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -370,187 +310,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,6 +517,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -586,17 +541,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -618,26 +567,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,168 +606,161 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -843,12 +783,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1170,13 +1104,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71428571428571" defaultRowHeight="15" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.71428571428571" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="33.8571428571429" style="5" customWidth="1"/>
     <col min="2" max="2" width="45.4285714285714" style="5" customWidth="1"/>
@@ -1239,135 +1173,25 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="5" t="s">
+    <row r="6" s="7" customFormat="1" spans="1:3">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="5" t="s">
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" s="7" customFormat="1" spans="1:3">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" s="7" customFormat="1" spans="1:3">
-      <c r="A14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" s="7" customFormat="1" spans="1:3">
-      <c r="A15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" s="7" customFormat="1" spans="1:3">
-      <c r="A16" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" s="7" customFormat="1" spans="1:3">
-      <c r="A17" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1410,10 +1234,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1421,10 +1245,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1432,10 +1256,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1477,10 +1301,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1488,10 +1312,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1499,10 +1323,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="5" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>5</v>
@@ -1510,10 +1334,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>5</v>
@@ -1521,10 +1345,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>5</v>
@@ -1572,10 +1396,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>5</v>
@@ -1583,10 +1407,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>

</xml_diff>